<commit_message>
update tanggal 8 jam 10
</commit_message>
<xml_diff>
--- a/excel/data_karyawan.xlsx
+++ b/excel/data_karyawan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kerja\Project Magang\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\stm_cuti\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{540D154F-9F9A-4FB3-9D0B-C76658C3290D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{314BE2D9-E79B-472E-86D5-5CE686F95CF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{1E31DAEF-5BB0-4D94-95EF-731F23FBE257}"/>
+    <workbookView xWindow="3864" yWindow="3432" windowWidth="17280" windowHeight="9072" xr2:uid="{1E31DAEF-5BB0-4D94-95EF-731F23FBE257}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="472">
   <si>
     <t>nik</t>
   </si>
@@ -966,19 +966,491 @@
     <t>Kadep</t>
   </si>
   <si>
-    <t>Martinus N.</t>
-  </si>
-  <si>
     <t>0440058</t>
   </si>
   <si>
     <t>TEAM KHUSUS</t>
   </si>
   <si>
-    <t>Alex Sardioko</t>
-  </si>
-  <si>
     <t>0540236</t>
+  </si>
+  <si>
+    <t>nama_jabatan</t>
+  </si>
+  <si>
+    <t>DIREKTUR</t>
+  </si>
+  <si>
+    <t>FINANCE CONTROLING</t>
+  </si>
+  <si>
+    <t>MANAGER</t>
+  </si>
+  <si>
+    <t>ASS. MANAGER</t>
+  </si>
+  <si>
+    <t>SUPERVISOR</t>
+  </si>
+  <si>
+    <t>SUPERVISOR   (INTERNAL AUDIT)</t>
+  </si>
+  <si>
+    <t>STAFF</t>
+  </si>
+  <si>
+    <t>INTERNAL CONTROLS (AUDIT) MANAGER</t>
+  </si>
+  <si>
+    <t>DESAIN GRAFIS / IT</t>
+  </si>
+  <si>
+    <t>SEKRETARIS</t>
+  </si>
+  <si>
+    <t>STAFF AP</t>
+  </si>
+  <si>
+    <t>STOREKEEPER</t>
+  </si>
+  <si>
+    <t>BUILDING MANAGER</t>
+  </si>
+  <si>
+    <t>SENIOR SUPERVISOR</t>
+  </si>
+  <si>
+    <t>RECEPTIONIST</t>
+  </si>
+  <si>
+    <t>CLEANING</t>
+  </si>
+  <si>
+    <t>GARDENING</t>
+  </si>
+  <si>
+    <t>GONDOLLA</t>
+  </si>
+  <si>
+    <t>CLEANER</t>
+  </si>
+  <si>
+    <t>WAITERS</t>
+  </si>
+  <si>
+    <t>OFFICE BOY</t>
+  </si>
+  <si>
+    <t>GA STAFF</t>
+  </si>
+  <si>
+    <t>SAFETY OFFICER SUPERVISOR</t>
+  </si>
+  <si>
+    <t>MESSENGER</t>
+  </si>
+  <si>
+    <t>SUPERVISOR LEGAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MANAGER</t>
+  </si>
+  <si>
+    <t>DRIVER</t>
+  </si>
+  <si>
+    <t>K3 STAFF</t>
+  </si>
+  <si>
+    <t>HR STAFF</t>
+  </si>
+  <si>
+    <t>DANRU
+REGU A</t>
+  </si>
+  <si>
+    <t>REGU B</t>
+  </si>
+  <si>
+    <t>DANRU
+REGU C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPERATOR SAFETY </t>
+  </si>
+  <si>
+    <t>ASS. CHIEF</t>
+  </si>
+  <si>
+    <t>REGU D</t>
+  </si>
+  <si>
+    <t>REGU A</t>
+  </si>
+  <si>
+    <t>REGU C</t>
+  </si>
+  <si>
+    <t>DANRU
+REGU B</t>
+  </si>
+  <si>
+    <t>DANRU
+REGU D</t>
+  </si>
+  <si>
+    <t>STAFF ADMIN</t>
+  </si>
+  <si>
+    <t>CHIEF TEKNIK</t>
+  </si>
+  <si>
+    <t>TEKNISI</t>
+  </si>
+  <si>
+    <t>MARTINUS N.</t>
+  </si>
+  <si>
+    <t>ALEX SARDIOKO</t>
+  </si>
+  <si>
+    <t>YURIZKA ENDRA</t>
+  </si>
+  <si>
+    <t>2540874</t>
+  </si>
+  <si>
+    <t>tanggal_masuk</t>
+  </si>
+  <si>
+    <t>2003/08/01</t>
+  </si>
+  <si>
+    <t>2004/01/02</t>
+  </si>
+  <si>
+    <t>2015/03/01</t>
+  </si>
+  <si>
+    <t>2020/12/07</t>
+  </si>
+  <si>
+    <t>2006/10/02</t>
+  </si>
+  <si>
+    <t>2016/04/01</t>
+  </si>
+  <si>
+    <t>2016/08/15</t>
+  </si>
+  <si>
+    <t>2022/09/26</t>
+  </si>
+  <si>
+    <t>2014/09/01</t>
+  </si>
+  <si>
+    <t>2023/10/11</t>
+  </si>
+  <si>
+    <t>2025/03/10</t>
+  </si>
+  <si>
+    <t>2017/05/06</t>
+  </si>
+  <si>
+    <t>2018/03/01</t>
+  </si>
+  <si>
+    <t>1993/06/02</t>
+  </si>
+  <si>
+    <t>2012/04/30</t>
+  </si>
+  <si>
+    <t>2019/07/08</t>
+  </si>
+  <si>
+    <t>2019/07/29</t>
+  </si>
+  <si>
+    <t>1991/04/01</t>
+  </si>
+  <si>
+    <t>2024/11/01</t>
+  </si>
+  <si>
+    <t>2014/12/01</t>
+  </si>
+  <si>
+    <t>2015/06/01</t>
+  </si>
+  <si>
+    <t>1992/06/13</t>
+  </si>
+  <si>
+    <t>2024/04/22</t>
+  </si>
+  <si>
+    <t>1995/11/01</t>
+  </si>
+  <si>
+    <t>2010/10/01</t>
+  </si>
+  <si>
+    <t>1992/01/01</t>
+  </si>
+  <si>
+    <t>2016/01/04</t>
+  </si>
+  <si>
+    <t>2016/11/01</t>
+  </si>
+  <si>
+    <t>2004/08/02</t>
+  </si>
+  <si>
+    <t>1995/11/15</t>
+  </si>
+  <si>
+    <t>2023/02/27</t>
+  </si>
+  <si>
+    <t>2019/10/01</t>
+  </si>
+  <si>
+    <t>2012/01/02</t>
+  </si>
+  <si>
+    <t>2013/05/01</t>
+  </si>
+  <si>
+    <t>2023/08/01</t>
+  </si>
+  <si>
+    <t>2018/11/01</t>
+  </si>
+  <si>
+    <t>2017/02/01</t>
+  </si>
+  <si>
+    <t>2017/12/06</t>
+  </si>
+  <si>
+    <t>2019/04/16</t>
+  </si>
+  <si>
+    <t>2018/11/19</t>
+  </si>
+  <si>
+    <t>2013/09/01</t>
+  </si>
+  <si>
+    <t>2016/10/17</t>
+  </si>
+  <si>
+    <t>2013/10/01</t>
+  </si>
+  <si>
+    <t>2018/01/08</t>
+  </si>
+  <si>
+    <t>2013/03/05</t>
+  </si>
+  <si>
+    <t>2013/02/01</t>
+  </si>
+  <si>
+    <t>2013/09/02</t>
+  </si>
+  <si>
+    <t>2025/01/13</t>
+  </si>
+  <si>
+    <t>2014/03/03</t>
+  </si>
+  <si>
+    <t>2017/08/14</t>
+  </si>
+  <si>
+    <t>2012/04/02</t>
+  </si>
+  <si>
+    <t>2016/05/02</t>
+  </si>
+  <si>
+    <t>2019/11/01</t>
+  </si>
+  <si>
+    <t>1990/12/17</t>
+  </si>
+  <si>
+    <t>2001/04/16</t>
+  </si>
+  <si>
+    <t>2013/06/03</t>
+  </si>
+  <si>
+    <t>2019/08/19</t>
+  </si>
+  <si>
+    <t>1996/03/05</t>
+  </si>
+  <si>
+    <t>2011/12/01</t>
+  </si>
+  <si>
+    <t>2020/02/03</t>
+  </si>
+  <si>
+    <t>2011/01/12</t>
+  </si>
+  <si>
+    <t>2005/06/01</t>
+  </si>
+  <si>
+    <t>2018/12/17</t>
+  </si>
+  <si>
+    <t>2016/10/03</t>
+  </si>
+  <si>
+    <t>2022/07/27</t>
+  </si>
+  <si>
+    <t>2006/10/09</t>
+  </si>
+  <si>
+    <t>2025/08/11</t>
+  </si>
+  <si>
+    <t>2015/01/26</t>
+  </si>
+  <si>
+    <t>2020/12/01</t>
+  </si>
+  <si>
+    <t>1999/10/01</t>
+  </si>
+  <si>
+    <t>2000/09/19</t>
+  </si>
+  <si>
+    <t>1996/02/26</t>
+  </si>
+  <si>
+    <t>1991/05/20</t>
+  </si>
+  <si>
+    <t>2018/10/01</t>
+  </si>
+  <si>
+    <t>2000/11/03</t>
+  </si>
+  <si>
+    <t>2014/04/01</t>
+  </si>
+  <si>
+    <t>2012/05/01</t>
+  </si>
+  <si>
+    <t>2025/01/28</t>
+  </si>
+  <si>
+    <t>2023/10/05</t>
+  </si>
+  <si>
+    <t>2024/08/26</t>
+  </si>
+  <si>
+    <t>2014/01/01</t>
+  </si>
+  <si>
+    <t>2011/08/01</t>
+  </si>
+  <si>
+    <t>1995/07/01</t>
+  </si>
+  <si>
+    <t>1992/02/01</t>
+  </si>
+  <si>
+    <t>2019/09/23</t>
+  </si>
+  <si>
+    <t>2025/01/20</t>
+  </si>
+  <si>
+    <t>2009/02/01</t>
+  </si>
+  <si>
+    <t>2022/07/04</t>
+  </si>
+  <si>
+    <t>2013/04/01</t>
+  </si>
+  <si>
+    <t>2012/10/15</t>
+  </si>
+  <si>
+    <t>2016/02/15</t>
+  </si>
+  <si>
+    <t>2023/05/15</t>
+  </si>
+  <si>
+    <t>2024/08/19</t>
+  </si>
+  <si>
+    <t>2016/06/01</t>
+  </si>
+  <si>
+    <t>2015/09/01</t>
+  </si>
+  <si>
+    <t>2007/11/01</t>
+  </si>
+  <si>
+    <t>2020/07/16</t>
+  </si>
+  <si>
+    <t>2025/01/23</t>
+  </si>
+  <si>
+    <t>2023/02/06</t>
+  </si>
+  <si>
+    <t>2020/08/03</t>
+  </si>
+  <si>
+    <t>2018/09/17</t>
+  </si>
+  <si>
+    <t>2021/01/04</t>
+  </si>
+  <si>
+    <t>1996/06/06</t>
+  </si>
+  <si>
+    <t>2019/01/03</t>
+  </si>
+  <si>
+    <t>2023/01/09</t>
+  </si>
+  <si>
+    <t>2011/09/15</t>
+  </si>
+  <si>
+    <t>2015/09/04</t>
+  </si>
+  <si>
+    <t>2019/06/17</t>
+  </si>
+  <si>
+    <t>2024/09/01</t>
+  </si>
+  <si>
+    <t>2023/11/01</t>
   </si>
 </sst>
 </file>
@@ -991,7 +1463,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* \-_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0######"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1040,8 +1512,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1138,13 +1617,58 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1158,7 +1682,7 @@
     <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1351,12 +1875,114 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="5" fillId="6" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="5" fillId="6" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="6" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1678,21 +2304,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4352ABBF-8B9D-490C-B2BD-039828137071}">
-  <dimension ref="A1:D156"/>
+  <dimension ref="A1:M157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A150" workbookViewId="0">
-      <selection activeCell="B162" sqref="B162"/>
+    <sheetView tabSelected="1" topLeftCell="D142" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F157" sqref="F157"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
@@ -1705,8 +2334,15 @@
       <c r="D1" s="20" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E1" s="67" t="s">
+        <v>314</v>
+      </c>
+      <c r="F1" s="67" t="s">
+        <v>361</v>
+      </c>
+      <c r="G1" s="105"/>
+    </row>
+    <row r="2" spans="1:13" ht="15" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
@@ -1719,8 +2355,15 @@
       <c r="D2" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E2" s="71" t="s">
+        <v>315</v>
+      </c>
+      <c r="F2" s="101" t="s">
+        <v>362</v>
+      </c>
+      <c r="G2" s="105"/>
+    </row>
+    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>2</v>
       </c>
@@ -1733,8 +2376,15 @@
       <c r="D3" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E3" s="71" t="s">
+        <v>316</v>
+      </c>
+      <c r="F3" s="69" t="s">
+        <v>363</v>
+      </c>
+      <c r="G3" s="105"/>
+    </row>
+    <row r="4" spans="1:13" ht="15" x14ac:dyDescent="0.3">
       <c r="A4" s="19">
         <v>1540759</v>
       </c>
@@ -1747,8 +2397,15 @@
       <c r="D4" s="20" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E4" s="73" t="s">
+        <v>317</v>
+      </c>
+      <c r="F4" s="69" t="s">
+        <v>364</v>
+      </c>
+      <c r="G4" s="105"/>
+    </row>
+    <row r="5" spans="1:13" ht="15" x14ac:dyDescent="0.3">
       <c r="A5" s="21">
         <v>2040846</v>
       </c>
@@ -1761,8 +2418,15 @@
       <c r="D5" s="20" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E5" s="71" t="s">
+        <v>318</v>
+      </c>
+      <c r="F5" s="69" t="s">
+        <v>365</v>
+      </c>
+      <c r="G5" s="105"/>
+    </row>
+    <row r="6" spans="1:13" ht="15" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="s">
         <v>3</v>
       </c>
@@ -1775,8 +2439,15 @@
       <c r="D6" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E6" s="72" t="s">
+        <v>319</v>
+      </c>
+      <c r="F6" s="102" t="s">
+        <v>366</v>
+      </c>
+      <c r="G6" s="105"/>
+    </row>
+    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
         <v>4</v>
       </c>
@@ -1789,8 +2460,15 @@
       <c r="D7" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="E7" s="72" t="s">
+        <v>320</v>
+      </c>
+      <c r="F7" s="104" t="s">
+        <v>367</v>
+      </c>
+      <c r="G7" s="105"/>
+    </row>
+    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.3">
       <c r="A8" s="24" t="s">
         <v>5</v>
       </c>
@@ -1803,8 +2481,15 @@
       <c r="D8" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E8" s="73" t="s">
+        <v>321</v>
+      </c>
+      <c r="F8" s="102" t="s">
+        <v>368</v>
+      </c>
+      <c r="G8" s="105"/>
+    </row>
+    <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.3">
       <c r="A9" s="25" t="s">
         <v>6</v>
       </c>
@@ -1817,8 +2502,15 @@
       <c r="D9" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E9" s="74" t="s">
+        <v>321</v>
+      </c>
+      <c r="F9" s="102" t="s">
+        <v>369</v>
+      </c>
+      <c r="G9" s="105"/>
+    </row>
+    <row r="10" spans="1:13" ht="45" x14ac:dyDescent="0.3">
       <c r="A10" s="22">
         <v>1440738</v>
       </c>
@@ -1831,8 +2523,16 @@
       <c r="D10" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E10" s="72" t="s">
+        <v>322</v>
+      </c>
+      <c r="F10" s="27" t="s">
+        <v>370</v>
+      </c>
+      <c r="G10" s="105"/>
+      <c r="M10" s="105"/>
+    </row>
+    <row r="11" spans="1:13" ht="15" x14ac:dyDescent="0.3">
       <c r="A11" s="27" t="s">
         <v>7</v>
       </c>
@@ -1845,8 +2545,15 @@
       <c r="D11" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E11" s="73" t="s">
+        <v>321</v>
+      </c>
+      <c r="F11" s="102" t="s">
+        <v>371</v>
+      </c>
+      <c r="G11" s="105"/>
+    </row>
+    <row r="12" spans="1:13" ht="15" x14ac:dyDescent="0.3">
       <c r="A12" s="27" t="s">
         <v>8</v>
       </c>
@@ -1859,8 +2566,15 @@
       <c r="D12" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="E12" s="73" t="s">
+        <v>319</v>
+      </c>
+      <c r="F12" s="102" t="s">
+        <v>372</v>
+      </c>
+      <c r="G12" s="105"/>
+    </row>
+    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.3">
       <c r="A13" s="19">
         <v>1740799</v>
       </c>
@@ -1873,8 +2587,15 @@
       <c r="D13" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E13" s="73" t="s">
+        <v>323</v>
+      </c>
+      <c r="F13" s="102" t="s">
+        <v>373</v>
+      </c>
+      <c r="G13" s="105"/>
+    </row>
+    <row r="14" spans="1:13" ht="15" x14ac:dyDescent="0.3">
       <c r="A14" s="28" t="s">
         <v>9</v>
       </c>
@@ -1887,8 +2608,15 @@
       <c r="D14" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E14" s="74" t="s">
+        <v>319</v>
+      </c>
+      <c r="F14" s="102" t="s">
+        <v>374</v>
+      </c>
+      <c r="G14" s="105"/>
+    </row>
+    <row r="15" spans="1:13" ht="15" x14ac:dyDescent="0.3">
       <c r="A15" s="24" t="s">
         <v>10</v>
       </c>
@@ -1901,8 +2629,15 @@
       <c r="D15" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E15" s="70" t="s">
+        <v>324</v>
+      </c>
+      <c r="F15" s="102" t="s">
+        <v>375</v>
+      </c>
+      <c r="G15" s="105"/>
+    </row>
+    <row r="16" spans="1:13" ht="15" x14ac:dyDescent="0.3">
       <c r="A16" s="24" t="s">
         <v>11</v>
       </c>
@@ -1915,8 +2650,15 @@
       <c r="D16" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E16" s="70" t="s">
+        <v>325</v>
+      </c>
+      <c r="F16" s="102" t="s">
+        <v>376</v>
+      </c>
+      <c r="G16" s="105"/>
+    </row>
+    <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A17" s="29" t="s">
         <v>12</v>
       </c>
@@ -1929,8 +2671,15 @@
       <c r="D17" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E17" s="75" t="s">
+        <v>321</v>
+      </c>
+      <c r="F17" s="102" t="s">
+        <v>377</v>
+      </c>
+      <c r="G17" s="105"/>
+    </row>
+    <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A18" s="29" t="s">
         <v>13</v>
       </c>
@@ -1943,8 +2692,15 @@
       <c r="D18" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E18" s="75" t="s">
+        <v>321</v>
+      </c>
+      <c r="F18" s="102" t="s">
+        <v>378</v>
+      </c>
+      <c r="G18" s="105"/>
+    </row>
+    <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A19" s="31" t="s">
         <v>14</v>
       </c>
@@ -1957,8 +2713,15 @@
       <c r="D19" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E19" s="76" t="s">
+        <v>319</v>
+      </c>
+      <c r="F19" s="102" t="s">
+        <v>379</v>
+      </c>
+      <c r="G19" s="105"/>
+    </row>
+    <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A20" s="33" t="s">
         <v>15</v>
       </c>
@@ -1971,8 +2734,15 @@
       <c r="D20" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E20" s="76" t="s">
+        <v>321</v>
+      </c>
+      <c r="F20" s="102" t="s">
+        <v>380</v>
+      </c>
+      <c r="G20" s="105"/>
+    </row>
+    <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A21" s="31" t="s">
         <v>16</v>
       </c>
@@ -1985,8 +2755,15 @@
       <c r="D21" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E21" s="76" t="s">
+        <v>319</v>
+      </c>
+      <c r="F21" s="102" t="s">
+        <v>381</v>
+      </c>
+      <c r="G21" s="105"/>
+    </row>
+    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A22" s="34">
         <v>1540763</v>
       </c>
@@ -1999,8 +2776,15 @@
       <c r="D22" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E22" s="76" t="s">
+        <v>321</v>
+      </c>
+      <c r="F22" s="102" t="s">
+        <v>382</v>
+      </c>
+      <c r="G22" s="105"/>
+    </row>
+    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A23" s="31" t="s">
         <v>17</v>
       </c>
@@ -2013,8 +2797,15 @@
       <c r="D23" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E23" s="76" t="s">
+        <v>326</v>
+      </c>
+      <c r="F23" s="102" t="s">
+        <v>383</v>
+      </c>
+      <c r="G23" s="105"/>
+    </row>
+    <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A24" s="35" t="s">
         <v>40</v>
       </c>
@@ -2027,8 +2818,12 @@
       <c r="D24" s="20" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E24" s="78" t="s">
+        <v>327</v>
+      </c>
+      <c r="G24" s="105"/>
+    </row>
+    <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A25" s="37" t="s">
         <v>42</v>
       </c>
@@ -2041,8 +2836,15 @@
       <c r="D25" s="20" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E25" s="77" t="s">
+        <v>324</v>
+      </c>
+      <c r="F25" s="102" t="s">
+        <v>384</v>
+      </c>
+      <c r="G25" s="105"/>
+    </row>
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.3">
       <c r="A26" s="28" t="s">
         <v>44</v>
       </c>
@@ -2055,8 +2857,15 @@
       <c r="D26" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E26" s="79" t="s">
+        <v>328</v>
+      </c>
+      <c r="F26" s="102" t="s">
+        <v>385</v>
+      </c>
+      <c r="G26" s="105"/>
+    </row>
+    <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A27" s="25" t="s">
         <v>46</v>
       </c>
@@ -2069,8 +2878,15 @@
       <c r="D27" s="20" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E27" s="79" t="s">
+        <v>317</v>
+      </c>
+      <c r="F27" s="102" t="s">
+        <v>396</v>
+      </c>
+      <c r="G27" s="105"/>
+    </row>
+    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A28" s="28" t="s">
         <v>48</v>
       </c>
@@ -2083,8 +2899,15 @@
       <c r="D28" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E28" s="79" t="s">
+        <v>329</v>
+      </c>
+      <c r="F28" s="102" t="s">
+        <v>386</v>
+      </c>
+      <c r="G28" s="105"/>
+    </row>
+    <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A29" s="28" t="s">
         <v>50</v>
       </c>
@@ -2097,8 +2920,15 @@
       <c r="D29" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="E29" s="79" t="s">
+        <v>319</v>
+      </c>
+      <c r="F29" s="102" t="s">
+        <v>387</v>
+      </c>
+      <c r="G29" s="105"/>
+    </row>
+    <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>52</v>
       </c>
@@ -2111,8 +2941,15 @@
       <c r="D30" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E30" s="80" t="s">
+        <v>330</v>
+      </c>
+      <c r="F30" s="102" t="s">
+        <v>388</v>
+      </c>
+      <c r="G30" s="105"/>
+    </row>
+    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
         <v>54</v>
       </c>
@@ -2125,8 +2962,15 @@
       <c r="D31" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E31" s="81" t="s">
+        <v>331</v>
+      </c>
+      <c r="F31" s="102" t="s">
+        <v>397</v>
+      </c>
+      <c r="G31" s="105"/>
+    </row>
+    <row r="32" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A32" s="38" t="s">
         <v>56</v>
       </c>
@@ -2139,8 +2983,15 @@
       <c r="D32" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E32" s="81" t="s">
+        <v>332</v>
+      </c>
+      <c r="F32" s="102" t="s">
+        <v>390</v>
+      </c>
+      <c r="G32" s="105"/>
+    </row>
+    <row r="33" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A33" s="38" t="s">
         <v>58</v>
       </c>
@@ -2153,8 +3004,15 @@
       <c r="D33" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="E33" s="81" t="s">
+        <v>330</v>
+      </c>
+      <c r="F33" s="102" t="s">
+        <v>391</v>
+      </c>
+      <c r="G33" s="105"/>
+    </row>
+    <row r="34" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
         <v>60</v>
       </c>
@@ -2167,8 +3025,15 @@
       <c r="D34" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E34" s="81" t="s">
+        <v>330</v>
+      </c>
+      <c r="F34" s="102" t="s">
+        <v>392</v>
+      </c>
+      <c r="G34" s="105"/>
+    </row>
+    <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A35" s="39" t="s">
         <v>62</v>
       </c>
@@ -2181,8 +3046,15 @@
       <c r="D35" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E35" s="81" t="s">
+        <v>332</v>
+      </c>
+      <c r="F35" s="102" t="s">
+        <v>393</v>
+      </c>
+      <c r="G35" s="105"/>
+    </row>
+    <row r="36" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A36" s="38" t="s">
         <v>64</v>
       </c>
@@ -2195,8 +3067,15 @@
       <c r="D36" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E36" s="81" t="s">
+        <v>332</v>
+      </c>
+      <c r="F36" s="102" t="s">
+        <v>394</v>
+      </c>
+      <c r="G36" s="105"/>
+    </row>
+    <row r="37" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A37" s="38" t="s">
         <v>66</v>
       </c>
@@ -2209,8 +3088,15 @@
       <c r="D37" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E37" s="81" t="s">
+        <v>333</v>
+      </c>
+      <c r="F37" s="102" t="s">
+        <v>395</v>
+      </c>
+      <c r="G37" s="105"/>
+    </row>
+    <row r="38" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A38" s="38" t="s">
         <v>68</v>
       </c>
@@ -2223,8 +3109,15 @@
       <c r="D38" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E38" s="81" t="s">
+        <v>330</v>
+      </c>
+      <c r="F38" s="102" t="s">
+        <v>393</v>
+      </c>
+      <c r="G38" s="105"/>
+    </row>
+    <row r="39" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A39" s="38" t="s">
         <v>70</v>
       </c>
@@ -2237,8 +3130,15 @@
       <c r="D39" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E39" s="81" t="s">
+        <v>330</v>
+      </c>
+      <c r="F39" s="102" t="s">
+        <v>398</v>
+      </c>
+      <c r="G39" s="105"/>
+    </row>
+    <row r="40" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A40" s="38" t="s">
         <v>72</v>
       </c>
@@ -2251,8 +3151,15 @@
       <c r="D40" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E40" s="81" t="s">
+        <v>331</v>
+      </c>
+      <c r="F40" s="102" t="s">
+        <v>399</v>
+      </c>
+      <c r="G40" s="105"/>
+    </row>
+    <row r="41" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A41" s="40" t="s">
         <v>74</v>
       </c>
@@ -2265,8 +3172,15 @@
       <c r="D41" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E41" s="81" t="s">
+        <v>333</v>
+      </c>
+      <c r="F41" s="102" t="s">
+        <v>400</v>
+      </c>
+      <c r="G41" s="105"/>
+    </row>
+    <row r="42" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A42" s="41">
         <v>1840813</v>
       </c>
@@ -2279,8 +3193,15 @@
       <c r="D42" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E42" s="81" t="s">
+        <v>330</v>
+      </c>
+      <c r="F42" s="102" t="s">
+        <v>401</v>
+      </c>
+      <c r="G42" s="105"/>
+    </row>
+    <row r="43" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A43" s="38" t="s">
         <v>77</v>
       </c>
@@ -2293,8 +3214,15 @@
       <c r="D43" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E43" s="81" t="s">
+        <v>333</v>
+      </c>
+      <c r="F43" s="102" t="s">
+        <v>402</v>
+      </c>
+      <c r="G43" s="105"/>
+    </row>
+    <row r="44" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A44" s="38" t="s">
         <v>79</v>
       </c>
@@ -2307,8 +3235,15 @@
       <c r="D44" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E44" s="81" t="s">
+        <v>330</v>
+      </c>
+      <c r="F44" s="102" t="s">
+        <v>399</v>
+      </c>
+      <c r="G44" s="105"/>
+    </row>
+    <row r="45" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A45" s="38" t="s">
         <v>81</v>
       </c>
@@ -2321,8 +3256,15 @@
       <c r="D45" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E45" s="81" t="s">
+        <v>331</v>
+      </c>
+      <c r="F45" s="102" t="s">
+        <v>398</v>
+      </c>
+      <c r="G45" s="105"/>
+    </row>
+    <row r="46" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A46" s="38" t="s">
         <v>83</v>
       </c>
@@ -2335,8 +3277,15 @@
       <c r="D46" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E46" s="81" t="s">
+        <v>333</v>
+      </c>
+      <c r="F46" s="102" t="s">
+        <v>412</v>
+      </c>
+      <c r="G46" s="105"/>
+    </row>
+    <row r="47" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A47" s="9" t="s">
         <v>85</v>
       </c>
@@ -2349,8 +3298,15 @@
       <c r="D47" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E47" s="81" t="s">
+        <v>330</v>
+      </c>
+      <c r="F47" s="102" t="s">
+        <v>403</v>
+      </c>
+      <c r="G47" s="105"/>
+    </row>
+    <row r="48" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A48" s="38" t="s">
         <v>87</v>
       </c>
@@ -2363,8 +3319,15 @@
       <c r="D48" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E48" s="81" t="s">
+        <v>332</v>
+      </c>
+      <c r="F48" s="102" t="s">
+        <v>404</v>
+      </c>
+      <c r="G48" s="105"/>
+    </row>
+    <row r="49" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A49" s="41" t="s">
         <v>89</v>
       </c>
@@ -2377,8 +3340,15 @@
       <c r="D49" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E49" s="81" t="s">
+        <v>330</v>
+      </c>
+      <c r="F49" s="102" t="s">
+        <v>400</v>
+      </c>
+      <c r="G49" s="105"/>
+    </row>
+    <row r="50" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A50" s="38" t="s">
         <v>91</v>
       </c>
@@ -2391,8 +3361,15 @@
       <c r="D50" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E50" s="81" t="s">
+        <v>330</v>
+      </c>
+      <c r="F50" s="102" t="s">
+        <v>405</v>
+      </c>
+      <c r="G50" s="105"/>
+    </row>
+    <row r="51" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A51" s="38" t="s">
         <v>93</v>
       </c>
@@ -2405,8 +3382,15 @@
       <c r="D51" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E51" s="81" t="s">
+        <v>330</v>
+      </c>
+      <c r="F51" s="102" t="s">
+        <v>406</v>
+      </c>
+      <c r="G51" s="105"/>
+    </row>
+    <row r="52" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A52" s="38" t="s">
         <v>95</v>
       </c>
@@ -2419,8 +3403,15 @@
       <c r="D52" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E52" s="81" t="s">
+        <v>319</v>
+      </c>
+      <c r="F52" s="102" t="s">
+        <v>404</v>
+      </c>
+      <c r="G52" s="105"/>
+    </row>
+    <row r="53" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A53" s="38" t="s">
         <v>97</v>
       </c>
@@ -2433,8 +3424,15 @@
       <c r="D53" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E53" s="81" t="s">
+        <v>330</v>
+      </c>
+      <c r="F53" s="102" t="s">
+        <v>394</v>
+      </c>
+      <c r="G53" s="105"/>
+    </row>
+    <row r="54" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A54" s="38" t="s">
         <v>99</v>
       </c>
@@ -2447,8 +3445,15 @@
       <c r="D54" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E54" s="81" t="s">
+        <v>330</v>
+      </c>
+      <c r="F54" s="102" t="s">
+        <v>407</v>
+      </c>
+      <c r="G54" s="105"/>
+    </row>
+    <row r="55" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A55" s="38" t="s">
         <v>101</v>
       </c>
@@ -2461,8 +3466,15 @@
       <c r="D55" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E55" s="81" t="s">
+        <v>330</v>
+      </c>
+      <c r="F55" s="102" t="s">
+        <v>408</v>
+      </c>
+      <c r="G55" s="105"/>
+    </row>
+    <row r="56" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A56" s="39" t="s">
         <v>103</v>
       </c>
@@ -2475,8 +3487,15 @@
       <c r="D56" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E56" s="81" t="s">
+        <v>330</v>
+      </c>
+      <c r="F56" s="102" t="s">
+        <v>409</v>
+      </c>
+      <c r="G56" s="105"/>
+    </row>
+    <row r="57" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A57" s="38" t="s">
         <v>105</v>
       </c>
@@ -2489,8 +3508,15 @@
       <c r="D57" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E57" s="81" t="s">
+        <v>330</v>
+      </c>
+      <c r="F57" s="102" t="s">
+        <v>410</v>
+      </c>
+      <c r="G57" s="105"/>
+    </row>
+    <row r="58" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A58" s="38" t="s">
         <v>107</v>
       </c>
@@ -2503,8 +3529,15 @@
       <c r="D58" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E58" s="81" t="s">
+        <v>331</v>
+      </c>
+      <c r="F58" s="102" t="s">
+        <v>370</v>
+      </c>
+      <c r="G58" s="105"/>
+    </row>
+    <row r="59" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A59" s="38" t="s">
         <v>109</v>
       </c>
@@ -2517,8 +3550,15 @@
       <c r="D59" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E59" s="81" t="s">
+        <v>321</v>
+      </c>
+      <c r="F59" s="102" t="s">
+        <v>410</v>
+      </c>
+      <c r="G59" s="105"/>
+    </row>
+    <row r="60" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A60" s="38" t="s">
         <v>111</v>
       </c>
@@ -2531,8 +3571,15 @@
       <c r="D60" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E60" s="81" t="s">
+        <v>333</v>
+      </c>
+      <c r="F60" s="102" t="s">
+        <v>411</v>
+      </c>
+      <c r="G60" s="105"/>
+    </row>
+    <row r="61" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A61" s="38" t="s">
         <v>113</v>
       </c>
@@ -2545,8 +3592,15 @@
       <c r="D61" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="E61" s="81" t="s">
+        <v>333</v>
+      </c>
+      <c r="F61" s="102" t="s">
+        <v>404</v>
+      </c>
+      <c r="G61" s="105"/>
+    </row>
+    <row r="62" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A62" s="11" t="s">
         <v>115</v>
       </c>
@@ -2559,8 +3613,15 @@
       <c r="D62" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E62" s="82" t="s">
+        <v>333</v>
+      </c>
+      <c r="F62" s="102" t="s">
+        <v>388</v>
+      </c>
+      <c r="G62" s="105"/>
+    </row>
+    <row r="63" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A63" s="38" t="s">
         <v>117</v>
       </c>
@@ -2573,8 +3634,15 @@
       <c r="D63" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="E63" s="81" t="s">
+        <v>333</v>
+      </c>
+      <c r="F63" s="102" t="s">
+        <v>364</v>
+      </c>
+      <c r="G63" s="105"/>
+    </row>
+    <row r="64" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A64" s="12" t="s">
         <v>119</v>
       </c>
@@ -2587,8 +3655,15 @@
       <c r="D64" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E64" s="83" t="s">
+        <v>334</v>
+      </c>
+      <c r="F64" s="102" t="s">
+        <v>413</v>
+      </c>
+      <c r="G64" s="105"/>
+    </row>
+    <row r="65" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A65" s="38" t="s">
         <v>121</v>
       </c>
@@ -2601,8 +3676,15 @@
       <c r="D65" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E65" s="84" t="s">
+        <v>334</v>
+      </c>
+      <c r="F65" s="102" t="s">
+        <v>414</v>
+      </c>
+      <c r="G65" s="105"/>
+    </row>
+    <row r="66" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A66" s="43" t="s">
         <v>123</v>
       </c>
@@ -2615,8 +3697,15 @@
       <c r="D66" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E66" s="83" t="s">
+        <v>334</v>
+      </c>
+      <c r="F66" s="102" t="s">
+        <v>415</v>
+      </c>
+      <c r="G66" s="105"/>
+    </row>
+    <row r="67" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A67" s="43" t="s">
         <v>125</v>
       </c>
@@ -2629,8 +3718,15 @@
       <c r="D67" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E67" s="83" t="s">
+        <v>321</v>
+      </c>
+      <c r="F67" s="102" t="s">
+        <v>416</v>
+      </c>
+      <c r="G67" s="105"/>
+    </row>
+    <row r="68" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A68" s="43" t="s">
         <v>127</v>
       </c>
@@ -2643,8 +3739,15 @@
       <c r="D68" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E68" s="83" t="s">
+        <v>334</v>
+      </c>
+      <c r="F68" s="102" t="s">
+        <v>417</v>
+      </c>
+      <c r="G68" s="105"/>
+    </row>
+    <row r="69" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A69" s="28" t="s">
         <v>129</v>
       </c>
@@ -2657,8 +3760,15 @@
       <c r="D69" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E69" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="F69" s="102" t="s">
+        <v>418</v>
+      </c>
+      <c r="G69" s="105"/>
+    </row>
+    <row r="70" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A70" s="25" t="s">
         <v>130</v>
       </c>
@@ -2671,8 +3781,15 @@
       <c r="D70" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E70" s="85" t="s">
+        <v>336</v>
+      </c>
+      <c r="F70" s="102" t="s">
+        <v>367</v>
+      </c>
+      <c r="G70" s="105"/>
+    </row>
+    <row r="71" spans="1:7" ht="30" x14ac:dyDescent="0.3">
       <c r="A71" s="25" t="s">
         <v>132</v>
       </c>
@@ -2685,8 +3802,15 @@
       <c r="D71" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E71" s="85" t="s">
+        <v>337</v>
+      </c>
+      <c r="F71" s="102" t="s">
+        <v>419</v>
+      </c>
+      <c r="G71" s="105"/>
+    </row>
+    <row r="72" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A72" s="28" t="s">
         <v>134</v>
       </c>
@@ -2699,8 +3823,15 @@
       <c r="D72" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E72" s="85" t="s">
+        <v>338</v>
+      </c>
+      <c r="F72" s="102" t="s">
+        <v>420</v>
+      </c>
+      <c r="G72" s="105"/>
+    </row>
+    <row r="73" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A73" s="28" t="s">
         <v>136</v>
       </c>
@@ -2713,8 +3844,15 @@
       <c r="D73" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E73" s="85" t="s">
+        <v>339</v>
+      </c>
+      <c r="F73" s="102" t="s">
+        <v>421</v>
+      </c>
+      <c r="G73" s="105"/>
+    </row>
+    <row r="74" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A74" s="25" t="s">
         <v>138</v>
       </c>
@@ -2727,8 +3865,15 @@
       <c r="D74" s="20" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E74" s="85" t="s">
+        <v>340</v>
+      </c>
+      <c r="F74" s="102" t="s">
+        <v>422</v>
+      </c>
+      <c r="G74" s="105"/>
+    </row>
+    <row r="75" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A75" s="28" t="s">
         <v>140</v>
       </c>
@@ -2741,8 +3886,15 @@
       <c r="D75" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E75" s="85" t="s">
+        <v>341</v>
+      </c>
+      <c r="F75" s="102" t="s">
+        <v>423</v>
+      </c>
+      <c r="G75" s="105"/>
+    </row>
+    <row r="76" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A76" s="44" t="s">
         <v>142</v>
       </c>
@@ -2755,8 +3907,15 @@
       <c r="D76" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E76" s="85" t="s">
+        <v>342</v>
+      </c>
+      <c r="F76" s="102" t="s">
+        <v>424</v>
+      </c>
+      <c r="G76" s="105"/>
+    </row>
+    <row r="77" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A77" s="9" t="s">
         <v>144</v>
       </c>
@@ -2769,8 +3928,15 @@
       <c r="D77" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E77" s="86" t="s">
+        <v>343</v>
+      </c>
+      <c r="F77" s="102" t="s">
+        <v>425</v>
+      </c>
+      <c r="G77" s="105"/>
+    </row>
+    <row r="78" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A78" s="25" t="s">
         <v>146</v>
       </c>
@@ -2783,8 +3949,15 @@
       <c r="D78" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E78" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="F78" s="102" t="s">
+        <v>426</v>
+      </c>
+      <c r="G78" s="105"/>
+    </row>
+    <row r="79" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A79" s="28" t="s">
         <v>148</v>
       </c>
@@ -2797,8 +3970,15 @@
       <c r="D79" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E79" s="85" t="s">
+        <v>341</v>
+      </c>
+      <c r="F79" s="102" t="s">
+        <v>427</v>
+      </c>
+      <c r="G79" s="105"/>
+    </row>
+    <row r="80" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A80" s="28" t="s">
         <v>150</v>
       </c>
@@ -2811,8 +3991,15 @@
       <c r="D80" s="20" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E80" s="85" t="s">
+        <v>343</v>
+      </c>
+      <c r="F80" s="102" t="s">
+        <v>428</v>
+      </c>
+      <c r="G80" s="105"/>
+    </row>
+    <row r="81" spans="1:7" ht="30" x14ac:dyDescent="0.3">
       <c r="A81" s="45" t="s">
         <v>152</v>
       </c>
@@ -2825,8 +4012,15 @@
       <c r="D81" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E81" s="92" t="s">
+        <v>344</v>
+      </c>
+      <c r="F81" s="102" t="s">
+        <v>429</v>
+      </c>
+      <c r="G81" s="105"/>
+    </row>
+    <row r="82" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A82" s="23" t="s">
         <v>154</v>
       </c>
@@ -2839,8 +4033,15 @@
       <c r="D82" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E82" s="88" t="s">
+        <v>345</v>
+      </c>
+      <c r="F82" s="102" t="s">
+        <v>430</v>
+      </c>
+      <c r="G82" s="105"/>
+    </row>
+    <row r="83" spans="1:7" ht="30" x14ac:dyDescent="0.3">
       <c r="A83" s="47" t="s">
         <v>156</v>
       </c>
@@ -2853,8 +4054,15 @@
       <c r="D83" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E83" s="93" t="s">
+        <v>346</v>
+      </c>
+      <c r="F83" s="102" t="s">
+        <v>431</v>
+      </c>
+      <c r="G83" s="105"/>
+    </row>
+    <row r="84" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A84" s="28" t="s">
         <v>158</v>
       </c>
@@ -2867,8 +4075,15 @@
       <c r="D84" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E84" s="87" t="s">
+        <v>347</v>
+      </c>
+      <c r="F84" s="102" t="s">
+        <v>432</v>
+      </c>
+      <c r="G84" s="105"/>
+    </row>
+    <row r="85" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A85" s="49" t="s">
         <v>160</v>
       </c>
@@ -2881,8 +4096,15 @@
       <c r="D85" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E85" s="94" t="s">
+        <v>348</v>
+      </c>
+      <c r="F85" s="102" t="s">
+        <v>433</v>
+      </c>
+      <c r="G85" s="105"/>
+    </row>
+    <row r="86" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A86" s="43" t="s">
         <v>162</v>
       </c>
@@ -2895,8 +4117,15 @@
       <c r="D86" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E86" s="88" t="s">
+        <v>349</v>
+      </c>
+      <c r="F86" s="102" t="s">
+        <v>434</v>
+      </c>
+      <c r="G86" s="105"/>
+    </row>
+    <row r="87" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A87" s="51" t="s">
         <v>164</v>
       </c>
@@ -2909,8 +4138,15 @@
       <c r="D87" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E87" s="88" t="s">
+        <v>350</v>
+      </c>
+      <c r="F87" s="102" t="s">
+        <v>435</v>
+      </c>
+      <c r="G87" s="105"/>
+    </row>
+    <row r="88" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A88" s="43" t="s">
         <v>166</v>
       </c>
@@ -2923,8 +4159,15 @@
       <c r="D88" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E88" s="89" t="s">
+        <v>351</v>
+      </c>
+      <c r="F88" s="102" t="s">
+        <v>436</v>
+      </c>
+      <c r="G88" s="105"/>
+    </row>
+    <row r="89" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A89" s="52" t="s">
         <v>168</v>
       </c>
@@ -2937,8 +4180,15 @@
       <c r="D89" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E89" s="88" t="s">
+        <v>349</v>
+      </c>
+      <c r="F89" s="102" t="s">
+        <v>430</v>
+      </c>
+      <c r="G89" s="105"/>
+    </row>
+    <row r="90" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A90" s="43" t="s">
         <v>170</v>
       </c>
@@ -2951,8 +4201,15 @@
       <c r="D90" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E90" s="89" t="s">
+        <v>350</v>
+      </c>
+      <c r="F90" s="102" t="s">
+        <v>430</v>
+      </c>
+      <c r="G90" s="105"/>
+    </row>
+    <row r="91" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A91" s="53" t="s">
         <v>172</v>
       </c>
@@ -2965,8 +4222,15 @@
       <c r="D91" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E91" s="89" t="s">
+        <v>351</v>
+      </c>
+      <c r="F91" s="102" t="s">
+        <v>389</v>
+      </c>
+      <c r="G91" s="105"/>
+    </row>
+    <row r="92" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A92" s="43" t="s">
         <v>174</v>
       </c>
@@ -2979,8 +4243,15 @@
       <c r="D92" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E92" s="89" t="s">
+        <v>351</v>
+      </c>
+      <c r="F92" s="102" t="s">
+        <v>433</v>
+      </c>
+      <c r="G92" s="105"/>
+    </row>
+    <row r="93" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A93" s="43" t="s">
         <v>176</v>
       </c>
@@ -2993,8 +4264,15 @@
       <c r="D93" s="20" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E93" s="89" t="s">
+        <v>351</v>
+      </c>
+      <c r="F93" s="102" t="s">
+        <v>437</v>
+      </c>
+      <c r="G93" s="105"/>
+    </row>
+    <row r="94" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A94" s="43" t="s">
         <v>178</v>
       </c>
@@ -3007,8 +4285,15 @@
       <c r="D94" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E94" s="88" t="s">
+        <v>345</v>
+      </c>
+      <c r="F94" s="102" t="s">
+        <v>437</v>
+      </c>
+      <c r="G94" s="105"/>
+    </row>
+    <row r="95" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A95" s="43" t="s">
         <v>180</v>
       </c>
@@ -3021,8 +4306,15 @@
       <c r="D95" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E95" s="89" t="s">
+        <v>351</v>
+      </c>
+      <c r="F95" s="102" t="s">
+        <v>438</v>
+      </c>
+      <c r="G95" s="105"/>
+    </row>
+    <row r="96" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A96" s="53" t="s">
         <v>182</v>
       </c>
@@ -3035,8 +4327,15 @@
       <c r="D96" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E96" s="88" t="s">
+        <v>345</v>
+      </c>
+      <c r="F96" s="102" t="s">
+        <v>389</v>
+      </c>
+      <c r="G96" s="105"/>
+    </row>
+    <row r="97" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A97" s="51" t="s">
         <v>184</v>
       </c>
@@ -3049,8 +4348,15 @@
       <c r="D97" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E97" s="89" t="s">
+        <v>345</v>
+      </c>
+      <c r="F97" s="102" t="s">
+        <v>389</v>
+      </c>
+      <c r="G97" s="105"/>
+    </row>
+    <row r="98" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A98" s="54" t="s">
         <v>8</v>
       </c>
@@ -3063,8 +4369,15 @@
       <c r="D98" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E98" s="89" t="s">
+        <v>350</v>
+      </c>
+      <c r="F98" s="102" t="s">
+        <v>439</v>
+      </c>
+      <c r="G98" s="105"/>
+    </row>
+    <row r="99" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A99" s="55" t="s">
         <v>187</v>
       </c>
@@ -3077,8 +4390,15 @@
       <c r="D99" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E99" s="89" t="s">
+        <v>351</v>
+      </c>
+      <c r="F99" s="102" t="s">
+        <v>440</v>
+      </c>
+      <c r="G99" s="105"/>
+    </row>
+    <row r="100" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A100" s="55" t="s">
         <v>189</v>
       </c>
@@ -3091,8 +4411,15 @@
       <c r="D100" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E100" s="89" t="s">
+        <v>351</v>
+      </c>
+      <c r="F100" s="102" t="s">
+        <v>441</v>
+      </c>
+      <c r="G100" s="105"/>
+    </row>
+    <row r="101" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A101" s="43" t="s">
         <v>191</v>
       </c>
@@ -3105,8 +4432,15 @@
       <c r="D101" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E101" s="89" t="s">
+        <v>350</v>
+      </c>
+      <c r="F101" s="102" t="s">
+        <v>438</v>
+      </c>
+      <c r="G101" s="105"/>
+    </row>
+    <row r="102" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A102" s="53" t="s">
         <v>193</v>
       </c>
@@ -3119,8 +4453,15 @@
       <c r="D102" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E102" s="88" t="s">
+        <v>345</v>
+      </c>
+      <c r="F102" s="102" t="s">
+        <v>418</v>
+      </c>
+      <c r="G102" s="105"/>
+    </row>
+    <row r="103" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A103" s="53" t="s">
         <v>195</v>
       </c>
@@ -3133,8 +4474,15 @@
       <c r="D103" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E103" s="88" t="s">
+        <v>349</v>
+      </c>
+      <c r="F103" s="102" t="s">
+        <v>393</v>
+      </c>
+      <c r="G103" s="105"/>
+    </row>
+    <row r="104" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A104" s="38" t="s">
         <v>197</v>
       </c>
@@ -3147,8 +4495,15 @@
       <c r="D104" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E104" s="88" t="s">
+        <v>349</v>
+      </c>
+      <c r="F104" s="102" t="s">
+        <v>442</v>
+      </c>
+      <c r="G104" s="105"/>
+    </row>
+    <row r="105" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A105" s="56" t="s">
         <v>199</v>
       </c>
@@ -3161,8 +4516,15 @@
       <c r="D105" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E105" s="88" t="s">
+        <v>345</v>
+      </c>
+      <c r="F105" s="102" t="s">
+        <v>443</v>
+      </c>
+      <c r="G105" s="105"/>
+    </row>
+    <row r="106" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A106" s="56" t="s">
         <v>201</v>
       </c>
@@ -3175,8 +4537,15 @@
       <c r="D106" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E106" s="88" t="s">
+        <v>350</v>
+      </c>
+      <c r="F106" s="102" t="s">
+        <v>444</v>
+      </c>
+      <c r="G106" s="105"/>
+    </row>
+    <row r="107" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A107" s="42" t="s">
         <v>203</v>
       </c>
@@ -3189,8 +4558,15 @@
       <c r="D107" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E107" s="88" t="s">
+        <v>345</v>
+      </c>
+      <c r="F107" s="102" t="s">
+        <v>429</v>
+      </c>
+      <c r="G107" s="105"/>
+    </row>
+    <row r="108" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A108" s="43" t="s">
         <v>205</v>
       </c>
@@ -3203,8 +4579,15 @@
       <c r="D108" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E108" s="89" t="s">
+        <v>351</v>
+      </c>
+      <c r="F108" s="102" t="s">
+        <v>430</v>
+      </c>
+      <c r="G108" s="105"/>
+    </row>
+    <row r="109" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A109" s="49" t="s">
         <v>207</v>
       </c>
@@ -3217,8 +4600,15 @@
       <c r="D109" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E109" s="94" t="s">
+        <v>348</v>
+      </c>
+      <c r="F109" s="102" t="s">
+        <v>445</v>
+      </c>
+      <c r="G109" s="105"/>
+    </row>
+    <row r="110" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A110" s="43" t="s">
         <v>209</v>
       </c>
@@ -3231,8 +4621,15 @@
       <c r="D110" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E110" s="89" t="s">
+        <v>351</v>
+      </c>
+      <c r="F110" s="102" t="s">
+        <v>446</v>
+      </c>
+      <c r="G110" s="105"/>
+    </row>
+    <row r="111" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A111" s="51" t="s">
         <v>211</v>
       </c>
@@ -3245,8 +4642,15 @@
       <c r="D111" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E111" s="89" t="s">
+        <v>350</v>
+      </c>
+      <c r="F111" s="102" t="s">
+        <v>418</v>
+      </c>
+      <c r="G111" s="105"/>
+    </row>
+    <row r="112" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A112" s="43" t="s">
         <v>213</v>
       </c>
@@ -3259,8 +4663,15 @@
       <c r="D112" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E112" s="88" t="s">
+        <v>349</v>
+      </c>
+      <c r="F112" s="102" t="s">
+        <v>443</v>
+      </c>
+      <c r="G112" s="105"/>
+    </row>
+    <row r="113" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A113" s="43" t="s">
         <v>215</v>
       </c>
@@ -3273,8 +4684,15 @@
       <c r="D113" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E113" s="89" t="s">
+        <v>350</v>
+      </c>
+      <c r="F113" s="102" t="s">
+        <v>445</v>
+      </c>
+      <c r="G113" s="105"/>
+    </row>
+    <row r="114" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A114" s="53" t="s">
         <v>217</v>
       </c>
@@ -3287,8 +4705,15 @@
       <c r="D114" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E114" s="88" t="s">
+        <v>350</v>
+      </c>
+      <c r="F114" s="102" t="s">
+        <v>418</v>
+      </c>
+      <c r="G114" s="105"/>
+    </row>
+    <row r="115" spans="1:7" ht="30" x14ac:dyDescent="0.3">
       <c r="A115" s="49" t="s">
         <v>219</v>
       </c>
@@ -3301,8 +4726,15 @@
       <c r="D115" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E115" s="94" t="s">
+        <v>352</v>
+      </c>
+      <c r="F115" s="102" t="s">
+        <v>433</v>
+      </c>
+      <c r="G115" s="105"/>
+    </row>
+    <row r="116" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A116" s="53" t="s">
         <v>221</v>
       </c>
@@ -3315,8 +4747,15 @@
       <c r="D116" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E116" s="88" t="s">
+        <v>345</v>
+      </c>
+      <c r="F116" s="102" t="s">
+        <v>435</v>
+      </c>
+      <c r="G116" s="105"/>
+    </row>
+    <row r="117" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A117" s="57" t="s">
         <v>223</v>
       </c>
@@ -3329,8 +4768,15 @@
       <c r="D117" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E117" s="88" t="s">
+        <v>349</v>
+      </c>
+      <c r="F117" s="102" t="s">
+        <v>447</v>
+      </c>
+      <c r="G117" s="105"/>
+    </row>
+    <row r="118" spans="1:7" ht="30" x14ac:dyDescent="0.3">
       <c r="A118" s="49" t="s">
         <v>225</v>
       </c>
@@ -3343,8 +4789,15 @@
       <c r="D118" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E118" s="94" t="s">
+        <v>353</v>
+      </c>
+      <c r="F118" s="102" t="s">
+        <v>448</v>
+      </c>
+      <c r="G118" s="105"/>
+    </row>
+    <row r="119" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A119" s="39" t="s">
         <v>227</v>
       </c>
@@ -3357,8 +4810,15 @@
       <c r="D119" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E119" s="90" t="s">
+        <v>354</v>
+      </c>
+      <c r="F119" s="102" t="s">
+        <v>449</v>
+      </c>
+      <c r="G119" s="105"/>
+    </row>
+    <row r="120" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A120" s="43" t="s">
         <v>229</v>
       </c>
@@ -3371,8 +4831,15 @@
       <c r="D120" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E120" s="89" t="s">
+        <v>350</v>
+      </c>
+      <c r="F120" s="102" t="s">
+        <v>450</v>
+      </c>
+      <c r="G120" s="105"/>
+    </row>
+    <row r="121" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A121" s="58" t="s">
         <v>231</v>
       </c>
@@ -3385,8 +4852,15 @@
       <c r="D121" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E121" s="95" t="s">
+        <v>345</v>
+      </c>
+      <c r="F121" s="102" t="s">
+        <v>448</v>
+      </c>
+      <c r="G121" s="105"/>
+    </row>
+    <row r="122" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A122" s="60" t="s">
         <v>233</v>
       </c>
@@ -3399,8 +4873,15 @@
       <c r="D122" s="20" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E122" s="91" t="s">
+        <v>317</v>
+      </c>
+      <c r="F122" s="102" t="s">
+        <v>451</v>
+      </c>
+      <c r="G122" s="105"/>
+    </row>
+    <row r="123" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A123" s="58" t="s">
         <v>235</v>
       </c>
@@ -3413,8 +4894,15 @@
       <c r="D123" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E123" s="88" t="s">
+        <v>349</v>
+      </c>
+      <c r="F123" s="102" t="s">
+        <v>393</v>
+      </c>
+      <c r="G123" s="105"/>
+    </row>
+    <row r="124" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A124" s="38" t="s">
         <v>237</v>
       </c>
@@ -3427,8 +4915,15 @@
       <c r="D124" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E124" s="88" t="s">
+        <v>351</v>
+      </c>
+      <c r="F124" s="102" t="s">
+        <v>431</v>
+      </c>
+      <c r="G124" s="105"/>
+    </row>
+    <row r="125" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A125" s="53" t="s">
         <v>239</v>
       </c>
@@ -3441,8 +4936,15 @@
       <c r="D125" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E125" s="88" t="s">
+        <v>349</v>
+      </c>
+      <c r="F125" s="102" t="s">
+        <v>452</v>
+      </c>
+      <c r="G125" s="105"/>
+    </row>
+    <row r="126" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A126" s="51" t="s">
         <v>241</v>
       </c>
@@ -3455,8 +4957,15 @@
       <c r="D126" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E126" s="89" t="s">
+        <v>350</v>
+      </c>
+      <c r="F126" s="102" t="s">
+        <v>413</v>
+      </c>
+      <c r="G126" s="105"/>
+    </row>
+    <row r="127" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A127" s="42" t="s">
         <v>243</v>
       </c>
@@ -3469,8 +4978,15 @@
       <c r="D127" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E127" s="88" t="s">
+        <v>349</v>
+      </c>
+      <c r="F127" s="102" t="s">
+        <v>429</v>
+      </c>
+      <c r="G127" s="105"/>
+    </row>
+    <row r="128" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A128" s="62" t="s">
         <v>245</v>
       </c>
@@ -3483,8 +4999,15 @@
       <c r="D128" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E128" s="88" t="s">
+        <v>345</v>
+      </c>
+      <c r="F128" s="102" t="s">
+        <v>453</v>
+      </c>
+      <c r="G128" s="105"/>
+    </row>
+    <row r="129" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A129" s="42" t="s">
         <v>247</v>
       </c>
@@ -3497,8 +5020,15 @@
       <c r="D129" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E129" s="88" t="s">
+        <v>349</v>
+      </c>
+      <c r="F129" s="102" t="s">
+        <v>429</v>
+      </c>
+      <c r="G129" s="105"/>
+    </row>
+    <row r="130" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A130" s="28" t="s">
         <v>249</v>
       </c>
@@ -3511,8 +5041,15 @@
       <c r="D130" s="20" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E130" s="97" t="s">
+        <v>355</v>
+      </c>
+      <c r="F130" s="102" t="s">
+        <v>437</v>
+      </c>
+      <c r="G130" s="105"/>
+    </row>
+    <row r="131" spans="1:7" ht="30" x14ac:dyDescent="0.3">
       <c r="A131" s="25" t="s">
         <v>251</v>
       </c>
@@ -3525,8 +5062,15 @@
       <c r="D131" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="132" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E131" s="97" t="s">
+        <v>356</v>
+      </c>
+      <c r="F131" s="102" t="s">
+        <v>454</v>
+      </c>
+      <c r="G131" s="105"/>
+    </row>
+    <row r="132" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A132" s="28" t="s">
         <v>253</v>
       </c>
@@ -3539,8 +5083,15 @@
       <c r="D132" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E132" s="97" t="s">
+        <v>356</v>
+      </c>
+      <c r="F132" s="102" t="s">
+        <v>455</v>
+      </c>
+      <c r="G132" s="105"/>
+    </row>
+    <row r="133" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A133" s="28" t="s">
         <v>255</v>
       </c>
@@ -3553,8 +5104,15 @@
       <c r="D133" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="134" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E133" s="97" t="s">
+        <v>356</v>
+      </c>
+      <c r="F133" s="102" t="s">
+        <v>456</v>
+      </c>
+      <c r="G133" s="105"/>
+    </row>
+    <row r="134" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A134" s="28" t="s">
         <v>257</v>
       </c>
@@ -3567,8 +5125,15 @@
       <c r="D134" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="135" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E134" s="97" t="s">
+        <v>356</v>
+      </c>
+      <c r="F134" s="102" t="s">
+        <v>457</v>
+      </c>
+      <c r="G134" s="105"/>
+    </row>
+    <row r="135" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A135" s="33" t="s">
         <v>259</v>
       </c>
@@ -3581,8 +5146,15 @@
       <c r="D135" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="136" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E135" s="98" t="s">
+        <v>356</v>
+      </c>
+      <c r="F135" s="102" t="s">
+        <v>458</v>
+      </c>
+      <c r="G135" s="105"/>
+    </row>
+    <row r="136" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A136" s="26" t="s">
         <v>261</v>
       </c>
@@ -3595,8 +5167,15 @@
       <c r="D136" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="137" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E136" s="97" t="s">
+        <v>356</v>
+      </c>
+      <c r="F136" s="102" t="s">
+        <v>404</v>
+      </c>
+      <c r="G136" s="105"/>
+    </row>
+    <row r="137" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A137" s="63">
         <v>2540869</v>
       </c>
@@ -3609,8 +5188,15 @@
       <c r="D137" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="138" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E137" s="97" t="s">
+        <v>356</v>
+      </c>
+      <c r="F137" s="102" t="s">
+        <v>459</v>
+      </c>
+      <c r="G137" s="105"/>
+    </row>
+    <row r="138" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A138" s="25" t="s">
         <v>264</v>
       </c>
@@ -3623,8 +5209,15 @@
       <c r="D138" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="139" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E138" s="97" t="s">
+        <v>356</v>
+      </c>
+      <c r="F138" s="102" t="s">
+        <v>460</v>
+      </c>
+      <c r="G138" s="105"/>
+    </row>
+    <row r="139" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A139" s="33" t="s">
         <v>266</v>
       </c>
@@ -3637,8 +5230,15 @@
       <c r="D139" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="140" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E139" s="98" t="s">
+        <v>356</v>
+      </c>
+      <c r="F139" s="102" t="s">
+        <v>461</v>
+      </c>
+      <c r="G139" s="105"/>
+    </row>
+    <row r="140" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A140" s="26">
         <v>1840810</v>
       </c>
@@ -3651,8 +5251,15 @@
       <c r="D140" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="141" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E140" s="97" t="s">
+        <v>356</v>
+      </c>
+      <c r="F140" s="102" t="s">
+        <v>462</v>
+      </c>
+      <c r="G140" s="105"/>
+    </row>
+    <row r="141" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A141" s="63" t="s">
         <v>269</v>
       </c>
@@ -3665,8 +5272,15 @@
       <c r="D141" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="142" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E141" s="97" t="s">
+        <v>356</v>
+      </c>
+      <c r="F141" s="102" t="s">
+        <v>460</v>
+      </c>
+      <c r="G141" s="105"/>
+    </row>
+    <row r="142" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A142" s="63" t="s">
         <v>271</v>
       </c>
@@ -3679,8 +5293,15 @@
       <c r="D142" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="143" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E142" s="97" t="s">
+        <v>356</v>
+      </c>
+      <c r="F142" s="102" t="s">
+        <v>463</v>
+      </c>
+      <c r="G142" s="105"/>
+    </row>
+    <row r="143" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A143" s="28" t="s">
         <v>273</v>
       </c>
@@ -3693,8 +5314,15 @@
       <c r="D143" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="144" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E143" s="97" t="s">
+        <v>356</v>
+      </c>
+      <c r="F143" s="102" t="s">
+        <v>464</v>
+      </c>
+      <c r="G143" s="105"/>
+    </row>
+    <row r="144" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A144" s="26">
         <v>1940815</v>
       </c>
@@ -3707,8 +5335,15 @@
       <c r="D144" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="145" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E144" s="97" t="s">
+        <v>356</v>
+      </c>
+      <c r="F144" s="102" t="s">
+        <v>465</v>
+      </c>
+      <c r="G144" s="105"/>
+    </row>
+    <row r="145" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A145" s="28" t="s">
         <v>276</v>
       </c>
@@ -3721,8 +5356,15 @@
       <c r="D145" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="146" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E145" s="97" t="s">
+        <v>356</v>
+      </c>
+      <c r="F145" s="102" t="s">
+        <v>457</v>
+      </c>
+      <c r="G145" s="105"/>
+    </row>
+    <row r="146" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A146" s="25" t="s">
         <v>278</v>
       </c>
@@ -3735,8 +5377,15 @@
       <c r="D146" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="147" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E146" s="97" t="s">
+        <v>356</v>
+      </c>
+      <c r="F146" s="102" t="s">
+        <v>466</v>
+      </c>
+      <c r="G146" s="105"/>
+    </row>
+    <row r="147" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A147" s="37" t="s">
         <v>280</v>
       </c>
@@ -3749,8 +5398,15 @@
       <c r="D147" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="148" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E147" s="96" t="s">
+        <v>356</v>
+      </c>
+      <c r="F147" s="102" t="s">
+        <v>461</v>
+      </c>
+      <c r="G147" s="105"/>
+    </row>
+    <row r="148" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A148" s="28" t="s">
         <v>282</v>
       </c>
@@ -3763,8 +5419,15 @@
       <c r="D148" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="149" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E148" s="97" t="s">
+        <v>319</v>
+      </c>
+      <c r="F148" s="102" t="s">
+        <v>467</v>
+      </c>
+      <c r="G148" s="105"/>
+    </row>
+    <row r="149" spans="1:7" ht="30" x14ac:dyDescent="0.3">
       <c r="A149" s="28" t="s">
         <v>284</v>
       </c>
@@ -3777,8 +5440,15 @@
       <c r="D149" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="150" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E149" s="97" t="s">
+        <v>328</v>
+      </c>
+      <c r="F149" s="102" t="s">
+        <v>468</v>
+      </c>
+      <c r="G149" s="105"/>
+    </row>
+    <row r="150" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A150" s="25" t="s">
         <v>286</v>
       </c>
@@ -3791,8 +5461,15 @@
       <c r="D150" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="151" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E150" s="97" t="s">
+        <v>319</v>
+      </c>
+      <c r="F150" s="102" t="s">
+        <v>438</v>
+      </c>
+      <c r="G150" s="105"/>
+    </row>
+    <row r="151" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A151" s="26" t="s">
         <v>288</v>
       </c>
@@ -3805,8 +5482,15 @@
       <c r="D151" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="152" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E151" s="97" t="s">
+        <v>356</v>
+      </c>
+      <c r="F151" s="102" t="s">
+        <v>469</v>
+      </c>
+      <c r="G151" s="105"/>
+    </row>
+    <row r="152" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A152" s="63" t="s">
         <v>290</v>
       </c>
@@ -3819,8 +5503,15 @@
       <c r="D152" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="153" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E152" s="99" t="s">
+        <v>356</v>
+      </c>
+      <c r="F152" s="102" t="s">
+        <v>470</v>
+      </c>
+      <c r="G152" s="105"/>
+    </row>
+    <row r="153" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A153" s="27" t="s">
         <v>292</v>
       </c>
@@ -3833,50 +5524,98 @@
       <c r="D153" s="20" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="154" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E153" s="100" t="s">
+        <v>354</v>
+      </c>
+      <c r="F153" s="102" t="s">
+        <v>471</v>
+      </c>
+      <c r="G153" s="105"/>
+    </row>
+    <row r="154" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A154" s="64" t="s">
+        <v>311</v>
+      </c>
+      <c r="B154" s="68" t="s">
+        <v>357</v>
+      </c>
+      <c r="C154" s="26" t="s">
         <v>312</v>
-      </c>
-      <c r="B154" s="65" t="s">
-        <v>311</v>
-      </c>
-      <c r="C154" s="26" t="s">
-        <v>313</v>
       </c>
       <c r="D154" s="20" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="155" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E154" s="26" t="s">
+        <v>319</v>
+      </c>
+      <c r="F154" s="102" t="s">
+        <v>467</v>
+      </c>
+      <c r="G154" s="103"/>
+    </row>
+    <row r="155" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A155" s="64" t="s">
-        <v>315</v>
-      </c>
-      <c r="B155" s="66" t="s">
-        <v>314</v>
+        <v>313</v>
+      </c>
+      <c r="B155" s="65" t="s">
+        <v>358</v>
       </c>
       <c r="C155" s="26" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D155" s="20" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="156" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A156" s="67" t="s">
+      <c r="E155" s="26" t="s">
+        <v>319</v>
+      </c>
+      <c r="F155" s="102" t="s">
+        <v>467</v>
+      </c>
+      <c r="G155" s="103"/>
+    </row>
+    <row r="156" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A156" s="69" t="s">
+        <v>360</v>
+      </c>
+      <c r="B156" t="s">
+        <v>359</v>
+      </c>
+      <c r="C156" s="26" t="s">
+        <v>298</v>
+      </c>
+      <c r="D156" s="67" t="s">
+        <v>310</v>
+      </c>
+      <c r="E156" s="26" t="s">
+        <v>319</v>
+      </c>
+      <c r="F156" s="102" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A157" s="66" t="s">
         <v>306</v>
       </c>
-      <c r="B156" s="6" t="s">
+      <c r="B157" s="6" t="s">
         <v>305</v>
       </c>
-      <c r="C156" s="26" t="s">
+      <c r="C157" s="26" t="s">
         <v>300</v>
       </c>
-      <c r="D156" s="20" t="s">
+      <c r="D157" s="20" t="s">
         <v>305</v>
+      </c>
+      <c r="E157" s="26" t="s">
+        <v>319</v>
+      </c>
+      <c r="F157" s="102" t="s">
+        <v>467</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>